<commit_message>
Upload new module with storage. Also, include the data files updated with this model: OG csv, A1 outputs, A2 extra inputs, A2 outputs
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Outputs/A-O_AR_Model_Base_Year.xlsx
+++ b/t1_confection/A1_Outputs/A-O_AR_Model_Base_Year.xlsx
@@ -1643,7 +1643,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4342,6 +4342,346 @@
       </c>
       <c r="J65" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>1</v>
+      </c>
+      <c r="B66" t="n">
+        <v/>
+      </c>
+      <c r="D66" t="n">
+        <v/>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>PWRBCKCRIXX</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Backstop (Power generator) Costa Rica, region XX</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>ELCCRIXX01</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>Electricity, Costa Rica, region XX, power plant output</t>
+        </is>
+      </c>
+      <c r="J66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>1</v>
+      </c>
+      <c r="B67" t="n">
+        <v/>
+      </c>
+      <c r="D67" t="n">
+        <v/>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>PWRBCKPANXX</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Backstop (Power generator) Panama, region XX</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>ELCPANXX01</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>Electricity, Panama, region XX, power plant output</t>
+        </is>
+      </c>
+      <c r="J67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>2</v>
+      </c>
+      <c r="B68" t="n">
+        <v/>
+      </c>
+      <c r="D68" t="n">
+        <v/>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>PWRLDSCRIXX01</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Long duration storage (Power generator) Costa Rica, region XX (can be invested) (Investable technology)</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>ELCCRIXX01</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>Electricity, Costa Rica, region XX, power plant output</t>
+        </is>
+      </c>
+      <c r="J68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>2</v>
+      </c>
+      <c r="B69" t="n">
+        <v/>
+      </c>
+      <c r="D69" t="n">
+        <v/>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>PWRLDSPANXX01</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Long duration storage (Power generator) Panama, region XX (can be invested) (Investable technology)</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>ELCPANXX01</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>Electricity, Panama, region XX, power plant output</t>
+        </is>
+      </c>
+      <c r="J69" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>2</v>
+      </c>
+      <c r="B70" t="n">
+        <v/>
+      </c>
+      <c r="D70" t="n">
+        <v/>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>PWRSDSCRIXX01</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Short duration storage (Power generator) Costa Rica, region XX (can be invested) (Investable technology)</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>ELCCRIXX01</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Electricity, Costa Rica, region XX, power plant output</t>
+        </is>
+      </c>
+      <c r="J70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>2</v>
+      </c>
+      <c r="B71" t="n">
+        <v/>
+      </c>
+      <c r="D71" t="n">
+        <v/>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>PWRSDSPANXX01</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Short duration storage (Power generator) Panama, region XX (can be invested) (Investable technology)</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>ELCPANXX01</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Electricity, Panama, region XX, power plant output</t>
+        </is>
+      </c>
+      <c r="J71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>1</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>ELCCRIXX01</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Electricity, Costa Rica, region XX, power plant output</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>1</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>PWRLDSCRIXX01</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Long duration storage (Power generator) Costa Rica, region XX (can be invested) (Investable technology)</t>
+        </is>
+      </c>
+      <c r="H72" t="n">
+        <v/>
+      </c>
+      <c r="J72" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>1</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>ELCPANXX01</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Electricity, Panama, region XX, power plant output</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>1</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>PWRLDSPANXX01</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Long duration storage (Power generator) Panama, region XX (can be invested) (Investable technology)</t>
+        </is>
+      </c>
+      <c r="H73" t="n">
+        <v/>
+      </c>
+      <c r="J73" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>1</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>ELCCRIXX01</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Electricity, Costa Rica, region XX, power plant output</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>1</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>PWRSDSCRIXX01</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Short duration storage (Power generator) Costa Rica, region XX (can be invested) (Investable technology)</t>
+        </is>
+      </c>
+      <c r="H74" t="n">
+        <v/>
+      </c>
+      <c r="J74" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>1</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>ELCPANXX01</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Electricity, Panama, region XX, power plant output</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>1</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>PWRSDSPANXX01</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Short duration storage (Power generator) Panama, region XX (can be invested) (Investable technology)</t>
+        </is>
+      </c>
+      <c r="H75" t="n">
+        <v/>
+      </c>
+      <c r="J75" t="n">
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>